<commit_message>
excel Airline test data added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
   <si>
     <t>testname</t>
   </si>
@@ -117,13 +118,139 @@
   </si>
   <si>
     <t>69.0</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Slogan</t>
+  </si>
+  <si>
+    <t>HeadQuarter</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Established</t>
+  </si>
+  <si>
+    <t>RandomNumber_6</t>
+  </si>
+  <si>
+    <t>AirlinePluto1</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Logo1</t>
+  </si>
+  <si>
+    <t>Slogan1</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Website1</t>
+  </si>
+  <si>
+    <t>AirlinePluto2</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Logo2</t>
+  </si>
+  <si>
+    <t>Slogan2</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Website2</t>
+  </si>
+  <si>
+    <t>RandomNumber</t>
+  </si>
+  <si>
+    <t>AirlinePluto3</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>Logo3</t>
+  </si>
+  <si>
+    <t>Slogan3</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Website3</t>
+  </si>
+  <si>
+    <t>RandomNumber_5</t>
+  </si>
+  <si>
+    <t>AirlinePluto4</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Logo4</t>
+  </si>
+  <si>
+    <t>Slogan4</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Website4</t>
+  </si>
+  <si>
+    <t>RandomNumber_4</t>
+  </si>
+  <si>
+    <t>AirlinePluto5</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Logo5</t>
+  </si>
+  <si>
+    <t>Slogan5</t>
+  </si>
+  <si>
+    <t>Shangai</t>
+  </si>
+  <si>
+    <t>Website5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,15 +266,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,15 +288,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,7 +374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,9 +406,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,6 +441,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -465,14 +617,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="101.21875" bestFit="1" customWidth="1"/>
@@ -481,7 +633,7 @@
     <col min="5" max="5" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -515,7 +667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -532,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -556,14 +708,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.21875" customWidth="1"/>
     <col min="2" max="3" width="18.109375" customWidth="1"/>
@@ -574,7 +726,7 @@
     <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +752,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -626,7 +778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -652,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -678,7 +830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -704,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -730,7 +882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -756,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -782,7 +934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34.049999999999997" customHeight="1">
+    <row r="9" spans="1:8" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -806,6 +958,180 @@
       </c>
       <c r="H9" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>5354366</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>